<commit_message>
Update Hospital_PowerBI_Project_Plan new (1).xlsx
</commit_message>
<xml_diff>
--- a/Hospital_PowerBI_Project_Plan new (1).xlsx
+++ b/Hospital_PowerBI_Project_Plan new (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ishan_IMP\GitHub Desktop files\Capstone_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F99F091-D038-417A-B5F3-89FF67CD0ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08336794-8D33-4295-BF01-4FDDA8F76E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="23040" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase_Task_Breakdown" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,17 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
- Create HospitalsAboveThreshold DAX
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Create HospitalsAboveThreshold DAX
 </t>
     </r>
     <r>
@@ -524,7 +534,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +560,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -590,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -603,6 +620,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -911,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,7 +1034,7 @@
       <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3">

</xml_diff>